<commit_message>
feat: Add the capacity to download excel reports, its being implemented the capacity to download csv reports
</commit_message>
<xml_diff>
--- a/server/output/Report.xlsx
+++ b/server/output/Report.xlsx
@@ -14,63 +14,39 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
-  <si>
-    <t>Nombres</t>
-  </si>
-  <si>
-    <t>Apellidos</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+  <si>
+    <t>ID</t>
   </si>
   <si>
     <t>Email</t>
   </si>
   <si>
-    <t>Creado el</t>
-  </si>
-  <si>
-    <t>Actualizado el</t>
-  </si>
-  <si>
-    <t>Marshall</t>
-  </si>
-  <si>
-    <t>Matters</t>
+    <t>23c0d5f8-17c9-4c92-b743-f662561e554f</t>
   </si>
   <si>
     <t/>
   </si>
   <si>
-    <t>Hannah 21</t>
-  </si>
-  <si>
-    <t>Wilson</t>
+    <t>19ca14e7-ace5-4d3b-8a6f-36ec768e9c5b</t>
   </si>
   <si>
     <t>hwilson@example.com</t>
   </si>
   <si>
-    <t>Voltereta</t>
-  </si>
-  <si>
-    <t>Ramirez</t>
+    <t>20be17b5-065c-4d88-a3a9-6167ead560b3</t>
   </si>
   <si>
     <t>VolteretaRamirez@gmai..com</t>
   </si>
   <si>
-    <t>Alice</t>
-  </si>
-  <si>
-    <t>Smith</t>
+    <t>2d7f68de-5c96-42ab-86c2-5b6b5c2f2c0d</t>
   </si>
   <si>
     <t>asmith@example.com</t>
   </si>
   <si>
-    <t>Bob</t>
-  </si>
-  <si>
-    <t>Williams</t>
+    <t>34ca6cf3-1748-4c71-b6a2-3b4f2c48d3a9</t>
   </si>
   <si>
     <t>bwilliams@example.com</t>
@@ -109,9 +85,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -451,109 +426,55 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:B6"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="B2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="B3" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>6</v>
       </c>
-      <c r="C2" t="s">
+      <c r="B4" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="1">
-        <v>45261.019791666666</v>
-      </c>
-      <c r="E2" s="1">
-        <v>45314.13605324074</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>8</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B5" t="s">
         <v>9</v>
       </c>
-      <c r="C3" t="s">
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="1">
-        <v>45261.019791666666</v>
-      </c>
-      <c r="E3" s="1">
-        <v>45314.13384259259</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="B6" t="s">
         <v>11</v>
-      </c>
-      <c r="B4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="1">
-        <v>45291.019791666666</v>
-      </c>
-      <c r="E4" s="1">
-        <v>45291.019791666666</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" s="1">
-        <v>45291.019791666666</v>
-      </c>
-      <c r="E5" s="1">
-        <v>45291.019791666666</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D6" s="1">
-        <v>45291.019791666666</v>
-      </c>
-      <c r="E6" s="1">
-        <v>45291.019791666666</v>
       </c>
     </row>
   </sheetData>

</xml_diff>